<commit_message>
videos script creation BDD
</commit_message>
<xml_diff>
--- a/03 - Databases/02 Exercice Videos/00-videos-Matrice-dépendances-fonctionnelles.xlsx
+++ b/03 - Databases/02 Exercice Videos/00-videos-Matrice-dépendances-fonctionnelles.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdevoldere\Documents\GitHub\DWWM_2409\03 - Databases\02 Exercice Videos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69FFD44-0F8B-4F9C-AB42-25B737CED6C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13430BA1-B907-45B6-A54B-5E0D3559D174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41295" yWindow="0" windowWidth="12810" windowHeight="14955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>Client_id</t>
   </si>
@@ -91,6 +92,39 @@
   </si>
   <si>
     <t>position_lecture</t>
+  </si>
+  <si>
+    <t>realisateur_id</t>
+  </si>
+  <si>
+    <t>realisateur_nom</t>
+  </si>
+  <si>
+    <t>Toto</t>
+  </si>
+  <si>
+    <t>Tata</t>
+  </si>
+  <si>
+    <t>Titi</t>
+  </si>
+  <si>
+    <t>film_id</t>
+  </si>
+  <si>
+    <t>film_titre</t>
+  </si>
+  <si>
+    <t>Léon</t>
+  </si>
+  <si>
+    <t>E.T</t>
+  </si>
+  <si>
+    <t>ça</t>
+  </si>
+  <si>
+    <t>Identity</t>
   </si>
 </sst>
 </file>
@@ -158,6 +192,29 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{06A10A3E-87EF-46D5-8EE0-3ED08901684E}" name="Tableau1" displayName="Tableau1" ref="D8:E11" totalsRowShown="0">
+  <autoFilter ref="D8:E11" xr:uid="{06A10A3E-87EF-46D5-8EE0-3ED08901684E}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{5211FF03-C4DB-445B-B5E4-F75C0115ED45}" name="realisateur_id"/>
+    <tableColumn id="2" xr3:uid="{C142F56F-568A-475D-8B21-F960D6C64711}" name="realisateur_nom"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5A6B7E6B-ECF8-4ADF-81D7-9610E7F7A832}" name="Tableau2" displayName="Tableau2" ref="G15:I19" totalsRowShown="0">
+  <autoFilter ref="G15:I19" xr:uid="{5A6B7E6B-ECF8-4ADF-81D7-9610E7F7A832}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{37D76F6E-53B9-4EA2-8C3C-865728EA80D2}" name="film_id"/>
+    <tableColumn id="2" xr3:uid="{4E2B8B74-40E1-40D9-A714-D8B09F4EBA23}" name="film_titre"/>
+    <tableColumn id="3" xr3:uid="{1F9EB1DD-7E0D-43E8-8EE6-A1DDFB50A97A}" name="realisateur_id"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -425,7 +482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -683,4 +740,117 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99571033-A785-4D9F-9E72-363135F46313}">
+  <dimension ref="D8:I19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>4</v>
+      </c>
+      <c r="H19" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>